<commit_message>
Added more test examples and cleanup
</commit_message>
<xml_diff>
--- a/src/test/resources/devices/devicelist.xlsx
+++ b/src/test/resources/devices/devicelist.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergio.barros/git/saucelabs-testng-example/src/test/resources/devices/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergio.barros/Workspace/git/testng-example/src/test/resources/devices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F10559-334B-7541-BA69-816C88C273CA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6796DE06-24B5-E947-BB26-D5046EA6A0E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32480" yWindow="-1140" windowWidth="21600" windowHeight="15940" tabRatio="345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20320" tabRatio="345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RealDevices" sheetId="5" r:id="rId1"/>
+    <sheet name="Browsers" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
   <si>
     <t>name</t>
   </si>
@@ -42,9 +43,6 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>testobject_device</t>
   </si>
   <si>
@@ -111,7 +109,55 @@
     <t>iPhone_7_11_4_real</t>
   </si>
   <si>
-    <t>1.9.1</t>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>chromeArguments</t>
+  </si>
+  <si>
+    <t>firefoxArguments</t>
+  </si>
+  <si>
+    <t>screenResolution</t>
+  </si>
+  <si>
+    <t>1.17.0</t>
+  </si>
+  <si>
+    <t>Windows 10</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>1280x960</t>
+  </si>
+  <si>
+    <t>SL_WIN10_CHROME_80</t>
+  </si>
+  <si>
+    <t>SL_WIN10_CHROME_79</t>
+  </si>
+  <si>
+    <t>SL_WIN10_CHROME_78</t>
+  </si>
+  <si>
+    <t>SL_WIN10_CHROME_77</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>77</t>
   </si>
 </sst>
 </file>
@@ -1431,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1454,10 +1500,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1469,118 +1515,118 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>28</v>
+      <c r="H2" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
+        <v>17</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -1591,34 +1637,34 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" t="b">
         <v>0</v>
@@ -1626,31 +1672,31 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -1661,34 +1707,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K7" t="b">
         <v>0</v>
@@ -1703,4 +1749,169 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF9C312-CD0B-024A-8448-6E3FC6249832}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
clean up and added combined execution of browser and device using different parallel config.
</commit_message>
<xml_diff>
--- a/src/test/resources/devices/devicelist.xlsx
+++ b/src/test/resources/devices/devicelist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergio.barros/Workspace/git/testng-example/src/test/resources/devices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6796DE06-24B5-E947-BB26-D5046EA6A0E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E85279C-A054-7A48-86B4-844C300D4A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20320" tabRatio="345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20320" tabRatio="345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RealDevices" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -158,6 +158,21 @@
   </si>
   <si>
     <t>77</t>
+  </si>
+  <si>
+    <t>supported</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -1475,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1495,7 +1510,7 @@
     <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1529,8 +1544,11 @@
       <c r="K1" t="s">
         <v>11</v>
       </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1564,8 +1582,11 @@
       <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1599,8 +1620,11 @@
       <c r="K3" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="L3" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1634,8 +1658,11 @@
       <c r="K4" t="b">
         <v>0</v>
       </c>
+      <c r="L4" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1652,7 +1679,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
@@ -1669,8 +1696,11 @@
       <c r="K5" t="b">
         <v>0</v>
       </c>
+      <c r="L5" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1704,8 +1734,11 @@
       <c r="K6" t="b">
         <v>0</v>
       </c>
+      <c r="L6" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1722,7 +1755,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
@@ -1738,6 +1771,9 @@
       </c>
       <c r="K7" t="b">
         <v>0</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1753,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF9C312-CD0B-024A-8448-6E3FC6249832}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1766,7 +1802,7 @@
     <col min="10" max="10" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1794,8 +1830,11 @@
       <c r="I1" t="s">
         <v>32</v>
       </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1823,8 +1862,11 @@
       <c r="I2" t="s">
         <v>36</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1852,8 +1894,11 @@
       <c r="I3" t="s">
         <v>36</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1881,8 +1926,11 @@
       <c r="I4" t="s">
         <v>36</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1909,6 +1957,9 @@
       </c>
       <c r="I5" t="s">
         <v>36</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added supported device support.
</commit_message>
<xml_diff>
--- a/src/test/resources/devices/devicelist.xlsx
+++ b/src/test/resources/devices/devicelist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergio.barros/Workspace/git/testng-example/src/test/resources/devices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E85279C-A054-7A48-86B4-844C300D4A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AE4FF6-4A72-8241-ABBC-74741DA6DB6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20320" tabRatio="345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -103,12 +103,6 @@
     <t/>
   </si>
   <si>
-    <t>Google_Pixel_XL_real</t>
-  </si>
-  <si>
-    <t>iPhone_7_11_4_real</t>
-  </si>
-  <si>
     <t>platform</t>
   </si>
   <si>
@@ -173,6 +167,12 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>Samsung_Galaxy_S10_real</t>
+  </si>
+  <si>
+    <t>iPhone_XS_13_real</t>
   </si>
 </sst>
 </file>
@@ -1493,7 +1493,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1545,15 +1545,15 @@
         <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -1571,7 +1571,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>24</v>
@@ -1579,19 +1579,19 @@
       <c r="J2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>24</v>
+      <c r="K2" t="b">
+        <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1609,7 +1609,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>24</v>
@@ -1617,11 +1617,11 @@
       <c r="J3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>24</v>
+      <c r="K3" t="b">
+        <v>0</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1647,7 +1647,7 @@
         <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>24</v>
@@ -1659,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1679,13 +1679,13 @@
         <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -1697,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1723,7 +1723,7 @@
         <v>22</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>24</v>
@@ -1735,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1755,13 +1755,13 @@
         <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -1773,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1792,7 +1792,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J2" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1810,48 +1810,48 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>24</v>
@@ -1860,30 +1860,30 @@
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>24</v>
@@ -1892,30 +1892,30 @@
         <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>24</v>
@@ -1924,30 +1924,30 @@
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>24</v>
@@ -1956,10 +1956,10 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>